<commit_message>
Update guide and questions grade 4
</commit_message>
<xml_diff>
--- a/Math_Data_Test.xlsx
+++ b/Math_Data_Test.xlsx
@@ -12368,28 +12368,115 @@
     <t>4 phút 25 giây = 255 giây.</t>
   </si>
   <si>
-    <t>To solve 'The average number of students in class 4A is 38. The number of students in class 4A is 6 less than in class 4B. The number of students in class 4A is:', subtract 6 from 38. The correct answer is 35.</t>
-  </si>
-  <si>
-    <t>Pour résoudre 'Le nombre moyen d'élèves dans la classe 4A est 38. Le nombre d'élèves dans la classe 4A est 6 de moins que dans la classe 4B. Le nombre d'élèves dans la classe 4A est :', soustrayez 6 de 38. La réponse correcte est 35.</t>
-  </si>
-  <si>
-    <t>Um 'Die durchschnittliche Schülerzahl in der Klasse 4A beträgt 38. Die Schülerzahl in der Klasse 4A ist um 6 Schüler weniger als in der Klasse 4B. Wie viele Schüler sind in der Klasse 4A?' zu lösen, subtrahiere 6 von 38. Die richtige Antwort ist 35.</t>
-  </si>
-  <si>
-    <t>Để giải 'Số học sinh trung bình trong lớp 4A là 38. Số học sinh trong lớp 4A ít hơn lớp 4B 6 học sinh. Số học sinh trong lớp 4A là:', trừ 6 từ 38. Đáp án đúng là 35.</t>
-  </si>
-  <si>
-    <t>The average number of students in class 4A is 38. The number of students in class 4A is 6 less than the number of students in class 4B. The number of students in class 4A is:</t>
-  </si>
-  <si>
-    <t>La moyenne du nombre d'élèves des deux classes 4A est de 38 élèves. Le nombre d'élèves dans la classe 4A est inférieur de 6 élèves à celui de la classe 4B. Le nombre d'élèves dans la classe 4A est :</t>
+    <t>Let the number of students in class 4A be x, and the number of students in class 4B be y. We have the following conditions:  
+The average number of students in the two classes is 38, which means:  
+(x + y)/2 = 38
+Multiplying both sides by 2:  
+x + y = 76
+The number of students in class 4A is 6 less than in class 4B, which means:  
+x = y - 6
+Substituting \( x = y - 6 \) into the equation \( x + y = 76 \):  
+(y - 6) + y = 76
+2y - 6 = 76
+2y = 82
+y = 41
+Thus,  
+x = 41 - 6 = 35
+So, the number of students in class 4A is 35.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soit \( x \) le nombre d'élèves de la classe 4A et \( y \) le nombre d'élèves de la classe 4B. Nous avons les conditions suivantes :  
+La moyenne du nombre d'élèves des deux classes est 38, ce qui signifie :  
+\[
+(x + y)/2 = 38
+\]
+En multipliant les deux côtés par 2 :  
+\[
+x + y = 76
+\]
+Le nombre d'élèves de la classe 4A est inférieur de 6 à celui de la classe 4B, soit :  
+\[
+x = y - 6
+\]
+En remplaçant \( x = y - 6 \) dans l'équation \( x + y = 76 \) :  
+\[
+(y - 6) + y = 76
+\]
+\[
+2y - 6 = 76
+\]
+\[
+2y = 82
+\]
+\[
+y = 41
+\]
+Ainsi,  
+\[
+x = 41 - 6 = 35
+\]
+Donc, le nombre d'élèves de la classe 4A est 35.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sei \( x \) die Anzahl der Schüler in Klasse 4A und \( y \) die Anzahl der Schüler in Klasse 4B. Wir haben die folgenden Bedingungen:  
+Der Durchschnitt der Schüleranzahl in beiden Klassen beträgt 38, das bedeutet:  
+\[
+(x + y)/2 = 38
+\]
+Multiplizieren beider Seiten mit 2:  
+\[
+x + y = 76
+\]
+Die Anzahl der Schüler in Klasse 4A ist um 6 kleiner als in Klasse 4B, also:  
+\[
+x = y - 6
+\]
+Setzen wir \( x = y - 6 \) in die Gleichung \( x + y = 76 \) ein:  
+\[
+(y - 6) + y = 76
+\]
+\[
+2y - 6 = 76
+\]
+\[
+2y = 82
+\]
+\[
+y = 41
+\]
+Daraus folgt:  
+\[
+x = 41 - 6 = 35
+\]
+Also beträgt die Anzahl der Schüler in Klasse 4A **35**.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gọi số học sinh của lớp 4A là \( x \), số học sinh của lớp 4B là \( y \). Ta có các điều kiện sau:  
+Trung bình cộng số học sinh của hai lớp là 38, tức là:  (x + y)/2 = 38
+  Nhân hai vế với 2:  x + y = 76
+  Số học sinh lớp 4A ít hơn số học sinh lớp 4B là 6 em, tức là:  x = y - 6
+Thay x = y - 6 vào phương trình x + y = 76:  
+(y - 6) + y = 76
+2y - 6 = 76
+2y = 82
+y = 41
+Suy ra x = 41 - 6 = 35.  
+Vậy số học sinh của lớp 4A là 35 em.
+</t>
+  </si>
+  <si>
+    <t>The average number of students in class 4 is 38. The number of students in class 4A is 6 less than the number of students in class 4B. The number of students in class 4A is:</t>
+  </si>
+  <si>
+    <t>La moyenne du nombre d'élèves des deux classes 4 est de 38 élèves. Le nombre d'élèves dans la classe 4A est inférieur de 6 élèves à celui de la classe 4B. Le nombre d'élèves dans la classe 4A est :</t>
   </si>
   <si>
     <t>Eine Kiste mit einem Gewicht von 8 kg ist voll mit Kartons, von denen jeder 2 kg wiegt. Wie viele Kartons befinden sich in der Kiste, wenn das Gewicht der Kiste 12 kg beträgt?</t>
   </si>
   <si>
-    <t>Trung bình cộng số học sinh của hai lớp 4A là 38 em. Số học sinh lớp 4A ít hơn số học sinh lớp 4B là 6 em. Số học sinh của lớp 4A là:</t>
+    <t>Trung bình cộng số học sinh của hai lớp 4 là 38 em. Số học sinh lớp 4A ít hơn số học sinh lớp 4B là 6 em. Số học sinh của lớp 4A là:</t>
   </si>
   <si>
     <t>M &lt; N</t>
@@ -12434,28 +12521,88 @@
     <t>M=N</t>
   </si>
   <si>
-    <t>To solve 'What's the largest value of the expression?', evaluate for the given range. The correct answer is 187.</t>
-  </si>
-  <si>
-    <t>Pour résoudre 'Quelle est la plus grande valeur de l'expression ?', évaluez pour l'intervalle donné. La réponse correcte est 187.</t>
-  </si>
-  <si>
-    <t>Um 'Was ist der größte Wert des Ausdrucks?' zu lösen, bewerte den gegebenen Wertebereich. Die richtige Antwort ist 187.</t>
-  </si>
-  <si>
-    <t>Để giải 'Giá trị lớn nhất của biểu thức là gì?', đánh giá cho khoảng giá trị đã cho. Đáp án đúng là 187.</t>
-  </si>
-  <si>
-    <t>Let's be different and all two-digit numbers. Most of the values ​​of the expression are:</t>
-  </si>
-  <si>
-    <t>Pour les nombres différents et tous à deux chiffres. La valeur maximale de l'expression est :</t>
-  </si>
-  <si>
-    <t>Gegeben sind verschiedene zweistellige Zahlen. Der größte Wert des Ausdrucks ist:</t>
-  </si>
-  <si>
-    <t>Cho là các số khác nhau và đều là số có hai chữ số. Giá trị lớn nhất của biểu thức là:</t>
+    <t xml:space="preserve">We need to find the maximum value of the expression: (x + y - 10) under the condition that  
+x and y are different numbers and both are two-digit numbers (i.e., from 10 to 99).  
+Step 1: Determine the value range of ( x + y )  
+The smallest value of ( x ) is 10, and the smallest value of ( y ) is 11 (since they must be different).  
+x + y = 10 + 11 = 21
+The largest value of ( x ) is 99, and the largest value of ( y ) is 98 (to keep them different).  
+x + y = 99 + 98 = 197
+Step 2: Find the maximum value of the expression  
+x + y - 10
+The maximum value is achieved when ( x + y ) is the largest, which means:  
+197 - 10 = 187
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nous devons trouver la valeur maximale de l'expression : \( x + y - 10 \) sous la condition que  
+\( x \) et \( y \) sont des nombres différents et qu'ils sont tous les deux des nombres à deux chiffres (c'est-à-dire de 10 à 99).  
+Étape 1 : Déterminer l'intervalle de valeurs de \( x + y \)  
+La plus petite valeur de \( x \) est 10, et la plus petite valeur de \( y \) est 11 (puisqu'ils doivent être différents).  
+\[
+x + y = 10 + 11 = 21
+\]
+La plus grande valeur de \( x \) est 99, et la plus grande valeur de \( y \) est 98 (pour qu'ils restent différents).  
+\[
+x + y = 99 + 98 = 197
+\]
+Étape 2 : Trouver la valeur maximale de l'expression  
+\[
+x + y - 10
+\]
+La valeur maximale est atteinte lorsque \( x + y \) est le plus grand, ce qui donne :  
+\[
+197 - 10 = 187
+\]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wir müssen den maximalen Wert des Ausdrucks \( x + y - 10 \) unter der Bedingung finden, dass  
+\( x \) und \( y \) unterschiedliche Zahlen sind und beide zweistellige Zahlen (d. h. von 10 bis 99) sind.  
+Schritt 1: Bestimmung des Wertebereichs von \( x + y \)  
+Der kleinste Wert von \( x \) ist 10, und der kleinste Wert von \( y \) ist 11 (da sie unterschiedlich sein müssen).  
+\[
+x + y = 10 + 11 = 21
+\]
+Der größte Wert von \( x \) ist 99, und der größte Wert von \( y \) ist 98 (um sie unterschiedlich zu halten).  
+\[
+x + y = 99 + 98 = 197
+\]
+Schritt 2: Bestimmung des maximalen Werts des Ausdrucks  
+\[
+x + y - 10
+\]
+Der maximale Wert wird erreicht, wenn \( x + y \) am größten ist, also:  
+\[
+197 - 10 = 187
+\]
+</t>
+  </si>
+  <si>
+    <t>Ta cần tìm giá trị lớn nhất của biểu thức: 𝑥 + 𝑦 − 10 với điều kiện 
+x và 𝑦 là các số khác nhau và đều là số có hai chữ số (tức là từ 10 đến 99).
+Bước 1: Xác định miền giá trị của 𝑥 + 𝑦
+Giá trị nhỏ nhất của x là 10, của y là 11 (vì chúng phải khác nhau).
+𝑥 + 𝑦 = 10 + 11 = 21
+Giá trị lớn nhất của x là 99, của y là 98 (để chúng khác nhau).
+𝑥 + 𝑦 = 99 + 98 = 197
+Bước 2: Tìm giá trị lớn nhất của biểu thức
+x+y−10
+Giá trị lớn nhất đạt được khi 
+x+y lớn nhất, tức là:
+197−10=187</t>
+  </si>
+  <si>
+    <t>Let's be different and all two-digit numbers. The maximum value of the expression x + y - 10 is:</t>
+  </si>
+  <si>
+    <t>Pour (x + y - 10), ce sont des nombres différents et tous deux sont des nombres à deux chiffres. La valeur maximale de l'expression est :</t>
+  </si>
+  <si>
+    <t>Gegeben ist, dass x + y - 10 verschiedene Zahlen sind und jeweils zweistellige Zahlen. Der größtmögliche Wert des Ausdrucks ist:</t>
+  </si>
+  <si>
+    <t>Cho x + y - 10 là các số khác nhau và đều là số có hai chữ số. Giá trị lớn nhất của biểu thức là:</t>
   </si>
   <si>
     <t>To solve 'With m = 6; n = 1086; p = 4. Calculate the value of the expression: p + m x n = ...', perform the multiplication and addition. The correct answer is 6520.</t>
@@ -58124,31 +58271,31 @@
       <c r="H1713" s="2">
         <v>2.0</v>
       </c>
-      <c r="I1713" s="2" t="s">
+      <c r="I1713" s="6" t="s">
         <v>3628</v>
       </c>
-      <c r="J1713" s="2" t="s">
+      <c r="J1713" s="6" t="s">
         <v>3629</v>
       </c>
-      <c r="K1713" s="2" t="s">
+      <c r="K1713" s="6" t="s">
         <v>3630</v>
       </c>
-      <c r="L1713" s="2" t="s">
+      <c r="L1713" s="6" t="s">
         <v>3631</v>
       </c>
       <c r="M1713" s="2">
         <v>28.0</v>
       </c>
-      <c r="N1713" s="2" t="s">
+      <c r="N1713" s="6" t="s">
         <v>3632</v>
       </c>
-      <c r="O1713" s="2" t="s">
+      <c r="O1713" s="6" t="s">
         <v>3633</v>
       </c>
       <c r="P1713" s="2" t="s">
         <v>3634</v>
       </c>
-      <c r="Q1713" s="2" t="s">
+      <c r="Q1713" s="6" t="s">
         <v>3635</v>
       </c>
     </row>
@@ -58296,31 +58443,31 @@
       <c r="H1721" s="2">
         <v>1.0</v>
       </c>
-      <c r="I1721" s="2" t="s">
+      <c r="I1721" s="6" t="s">
         <v>3650</v>
       </c>
-      <c r="J1721" s="2" t="s">
+      <c r="J1721" s="6" t="s">
         <v>3651</v>
       </c>
-      <c r="K1721" s="2" t="s">
+      <c r="K1721" s="6" t="s">
         <v>3652</v>
       </c>
-      <c r="L1721" s="2" t="s">
+      <c r="L1721" s="6" t="s">
         <v>3653</v>
       </c>
       <c r="M1721" s="2">
         <v>30.0</v>
       </c>
-      <c r="N1721" s="2" t="s">
+      <c r="N1721" s="6" t="s">
         <v>3654</v>
       </c>
-      <c r="O1721" s="2" t="s">
+      <c r="O1721" s="6" t="s">
         <v>3655</v>
       </c>
-      <c r="P1721" s="2" t="s">
+      <c r="P1721" s="6" t="s">
         <v>3656</v>
       </c>
-      <c r="Q1721" s="2" t="s">
+      <c r="Q1721" s="6" t="s">
         <v>3657</v>
       </c>
     </row>

</xml_diff>